<commit_message>
Added basic graph functionality for top ten domains,ip sources and query types
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -467,12 +467,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-03-05 12:40:21.124141</t>
+          <t>2025-03-05 17:28:24.329449</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>fd31:1623:3a00:148:ecbd:c962:c5d8:9b0b</t>
+          <t>fd31:1623:3a00:148:3554:8d02:4013:d1aa</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -482,11 +482,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>mobile.events.data.microsoft.com.</t>
+          <t>github.com.</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Spike chart for traffic
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,26 +467,251 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-03-05 17:28:24.329449</t>
+          <t>2025-03-05 20:11:04.332923</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>fd31:1623:3a00:148:3554:8d02:4013:d1aa</t>
+          <t>fd31:1623:3a00:148:200:3ff:fe88:f</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>fd31:1623:3a00:148:200:3ff:fe88:f</t>
+          <t>fd31:1623:3a00:148:3554:8d02:4013:d1aa</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>github.com.</t>
+          <t>audio-ak.spotifycdn.com.</t>
         </is>
       </c>
       <c r="E2" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-03-05 20:11:04.332923</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:200:3ff:fe88:f</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:3554:8d02:4013:d1aa</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>audio-ak.spotifycdn.com.</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-03-05 20:11:12.028097</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:3554:8d02:4013:d1aa</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:200:3ff:fe88:f</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>array602.prod.do.dsp.mp.microsoft.com.</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-03-05 20:11:12.056478</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:200:3ff:fe88:f</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:3554:8d02:4013:d1aa</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>array602.prod.do.dsp.mp.microsoft.com.</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-03-05 20:11:39.283269</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:3554:8d02:4013:d1aa</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:200:3ff:fe88:f</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>accounts.google.com.</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-03-05 20:11:39.283515</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:3554:8d02:4013:d1aa</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:200:3ff:fe88:f</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>accounts.google.com.</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-03-05 20:11:39.283676</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:3554:8d02:4013:d1aa</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:200:3ff:fe88:f</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>accounts.google.com.</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-03-05 20:11:39.311973</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:200:3ff:fe88:f</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:3554:8d02:4013:d1aa</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>accounts.google.com.</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-03-05 20:11:39.311973</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:200:3ff:fe88:f</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:3554:8d02:4013:d1aa</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>accounts.google.com.</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-03-05 20:11:39.317189</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:200:3ff:fe88:f</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>fd31:1623:3a00:148:3554:8d02:4013:d1aa</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>accounts.google.com.</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>